<commit_message>
add activate DND mode script and reduce wait from coappand guarantor xlsx sheet
</commit_message>
<xml_diff>
--- a/DataSheet/FOS3UW_to_postSanction2.xlsx
+++ b/DataSheet/FOS3UW_to_postSanction2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\biswa\eclipse-workspace\BSA_MOBILE_FRAMEWORK\DataSheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FC64CB2-56A8-4820-890A-ED8CBD27078D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6D82460-AC6B-439C-B1A3-CE94296DA13F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{875AE543-1650-41B3-9C38-4B818EB686AA}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{875AE543-1650-41B3-9C38-4B818EB686AA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1007,7 +1007,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC0CA32F-6895-4985-AF4D-119BC41D4938}">
   <dimension ref="A1:O229"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B155" zoomScale="74" workbookViewId="0">
+    <sheetView topLeftCell="B155" zoomScale="74" workbookViewId="0">
       <selection activeCell="H159" sqref="H159"/>
     </sheetView>
   </sheetViews>
@@ -8428,8 +8428,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41A86AEA-BDCA-4ACF-93E7-52FBBDAF5EE7}">
   <dimension ref="A1:Z3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M11" sqref="M11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8552,16 +8552,16 @@
         <v>1</v>
       </c>
       <c r="F2">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="G2">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="H2">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="I2">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="J2" s="4" t="s">
         <v>80</v>

</xml_diff>